<commit_message>
update to handle genRowFlag to set which rows to generate in from spreadsheet
</commit_message>
<xml_diff>
--- a/test/data/spreadsheet/sample.xlsx
+++ b/test/data/spreadsheet/sample.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wendylam/projects/data-file-generator/test/data/spreadsheet/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7DBD8B-5282-C34C-8340-B41CDFEF61F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="880" windowWidth="24720" windowHeight="15060" tabRatio="500"/>
+    <workbookView xWindow="8200" yWindow="800" windowWidth="24720" windowHeight="15060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="31">
   <si>
     <t>UNIQUE_ID_COLUMN</t>
   </si>
@@ -105,12 +111,21 @@
   </si>
   <si>
     <t>Matched2</t>
+  </si>
+  <si>
+    <t>GEN_ROW</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -122,6 +137,7 @@
     <font>
       <sz val="9"/>
       <name val="Menlo"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -216,6 +232,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -540,80 +564,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5" customWidth="1"/>
-    <col min="7" max="12" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="8" max="13" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G2" s="2" t="s">
         <v>22</v>
       </c>
@@ -623,34 +651,37 @@
       <c r="I2" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>23</v>
+      <c r="I3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>23</v>
@@ -658,30 +689,34 @@
       <c r="L3" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="4"/>
       <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
         <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -697,21 +732,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,7 +757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -733,7 +768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
@@ -744,7 +779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -766,20 +801,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,7 +822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>

</xml_diff>